<commit_message>
improve readability 100% zoom, fix potential spelling errors
</commit_message>
<xml_diff>
--- a/documents/sprint1_deliverables/Risk_Register.xlsx
+++ b/documents/sprint1_deliverables/Risk_Register.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aidan\Desktop\Sprint 1 deliverables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devops1\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{00FBD99C-7FA6-4F3C-84E5-DAF7B520BC09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEAB7FB0-9375-4071-99C5-CE6329630D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B2F38711-E786-4E3C-BFBF-4335729CB9FE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{B2F38711-E786-4E3C-BFBF-4335729CB9FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="107">
   <si>
     <t>Risk register</t>
   </si>
@@ -290,24 +279,15 @@
     <t>Budget of requirements yet to be done by client.</t>
   </si>
   <si>
-    <t>Data compatability issues</t>
-  </si>
-  <si>
     <t>Scalability and performance</t>
   </si>
   <si>
     <t>Data quality issues</t>
   </si>
   <si>
-    <t xml:space="preserve">Differences in document formats may cause compatability issues with incorrect processing or loss of information. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Technical, Information </t>
   </si>
   <si>
-    <t>Implement compatability testing for different documents and versions, may not be required as assuming we are only using docx files.</t>
-  </si>
-  <si>
     <t>In progress. No tests conducted as of now.</t>
   </si>
   <si>
@@ -323,15 +303,9 @@
     <t>Not implemented. Scalability tests in phase 3 after first revision.</t>
   </si>
   <si>
-    <t>Incomplete information / incorrect information could lead to inaccurate results of the application. Includes mainly incosistent or missing RSID codes</t>
-  </si>
-  <si>
     <t>Information, Quality</t>
   </si>
   <si>
-    <t>Not likeyl</t>
-  </si>
-  <si>
     <t xml:space="preserve">Implement data validation and cleansing process of input data. </t>
   </si>
   <si>
@@ -360,6 +334,18 @@
   </si>
   <si>
     <t>Risk status: Communicate the status of the task, Open, in progress, and closed.</t>
+  </si>
+  <si>
+    <t>Implement compatibility testing for different documents and versions, may not be required as assuming we are only using docx files.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Differences in document formats may cause compatibility issues with incorrect processing or loss of information. </t>
+  </si>
+  <si>
+    <t>Data compatibility issues</t>
+  </si>
+  <si>
+    <t>Incomplete information / incorrect information could lead to inaccurate results of the application. Includes mainly inconsistent or missing RSID codes</t>
   </si>
 </sst>
 </file>
@@ -439,24 +425,44 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -794,512 +800,519 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{343CE794-F272-4510-B09A-18E066DDE918}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="99.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="255.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="231.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="145" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.36328125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="37.6328125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="13" style="11" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" style="11" customWidth="1"/>
+    <col min="5" max="5" width="8.26953125" style="11" customWidth="1"/>
+    <col min="6" max="6" width="34.36328125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.54296875" style="13" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19.5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="19.5" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="7"/>
+    </row>
+    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+    <row r="14" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="130.5" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="13" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+      <c r="A18" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+      <c r="A22" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G22" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A24" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G25" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+      <c r="A27" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H27" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A28" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="G28" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="87" x14ac:dyDescent="0.35">
+      <c r="A29" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" t="s">
-        <v>16</v>
-      </c>
-      <c r="H15" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G16" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C17" t="s">
-        <v>26</v>
-      </c>
-      <c r="D17" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="C30" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E30" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="F30" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="G30" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" t="s">
-        <v>34</v>
-      </c>
-      <c r="E18" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" t="s">
-        <v>14</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G20" t="s">
-        <v>29</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" t="s">
-        <v>27</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G21" t="s">
-        <v>16</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" t="s">
-        <v>54</v>
-      </c>
-      <c r="D22" t="s">
-        <v>55</v>
-      </c>
-      <c r="E22" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G22" t="s">
-        <v>29</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C23" t="s">
-        <v>44</v>
-      </c>
-      <c r="D23" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G23" t="s">
-        <v>29</v>
-      </c>
-      <c r="H23" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D24" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" t="s">
-        <v>65</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C25" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" t="s">
-        <v>34</v>
-      </c>
-      <c r="E25" t="s">
-        <v>27</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G25" t="s">
-        <v>29</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" t="s">
-        <v>76</v>
-      </c>
-      <c r="D26" t="s">
-        <v>34</v>
-      </c>
-      <c r="E26" t="s">
-        <v>65</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G26" t="s">
-        <v>29</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C27" t="s">
-        <v>81</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E27" t="s">
-        <v>65</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G27" t="s">
-        <v>29</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" t="s">
-        <v>88</v>
-      </c>
-      <c r="D28" t="s">
-        <v>55</v>
-      </c>
-      <c r="E28" t="s">
-        <v>27</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="G28" t="s">
-        <v>29</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C29" t="s">
-        <v>92</v>
-      </c>
-      <c r="D29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" t="s">
-        <v>14</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="G29" t="s">
-        <v>16</v>
-      </c>
-      <c r="H29" s="3" t="s">
+      <c r="H30" s="6" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D30" t="s">
-        <v>97</v>
-      </c>
-      <c r="E30" t="s">
-        <v>27</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="G30" t="s">
-        <v>29</v>
-      </c>
-      <c r="H30" s="3" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>